<commit_message>
push lstm and 5 min data code
</commit_message>
<xml_diff>
--- a/results/5min/largest_window.xlsx
+++ b/results/5min/largest_window.xlsx
@@ -482,7 +482,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8538662940263748</v>
+        <v>0.9902682024985552</v>
       </c>
       <c r="G2" t="n">
         <v>57</v>
@@ -505,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9219675436615944</v>
+        <v>0.9524596519768238</v>
       </c>
       <c r="G3" t="n">
         <v>18</v>
@@ -528,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9620594792068005</v>
+        <v>0.9379133321344852</v>
       </c>
       <c r="G4" t="n">
         <v>47</v>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7974866181612015</v>
+        <v>0.9486318528652191</v>
       </c>
       <c r="G5" t="n">
         <v>123</v>
@@ -574,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6918849647045135</v>
+        <v>0.9907087041065097</v>
       </c>
       <c r="G6" t="n">
         <v>172</v>
@@ -597,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8600957244634628</v>
+        <v>0.9975055702961981</v>
       </c>
       <c r="G7" t="n">
         <v>34</v>
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8884619176387787</v>
+        <v>0.9927204083651304</v>
       </c>
       <c r="G8" t="n">
         <v>38</v>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8345680236816406</v>
+        <v>0.9908512523397803</v>
       </c>
       <c r="G9" t="n">
         <v>65</v>
@@ -666,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8764264732599258</v>
+        <v>0.9800759553909302</v>
       </c>
       <c r="G10" t="n">
         <v>61</v>
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8794823586940765</v>
+        <v>0.99901595688425</v>
       </c>
       <c r="G11" t="n">
         <v>20</v>
@@ -712,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5487156510353088</v>
+        <v>0.9577311463654041</v>
       </c>
       <c r="G12" t="n">
         <v>122</v>
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8609542995691299</v>
+        <v>0.9606174230575562</v>
       </c>
       <c r="G13" t="n">
         <v>116</v>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8991541936993599</v>
+        <v>0.9980188477784395</v>
       </c>
       <c r="G14" t="n">
         <v>162</v>
@@ -781,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9202811494469643</v>
+        <v>0.9295283704996109</v>
       </c>
       <c r="G15" t="n">
         <v>104</v>
@@ -804,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6698240041732788</v>
+        <v>0.9929364589042962</v>
       </c>
       <c r="G16" t="n">
         <v>99</v>
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9904404785484076</v>
+        <v>0.6725634336471558</v>
       </c>
       <c r="G17" t="n">
         <v>20</v>
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7715707272291183</v>
+        <v>0.9918723702430725</v>
       </c>
       <c r="G18" t="n">
         <v>123</v>
@@ -873,7 +873,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9841150157153606</v>
+        <v>0.9409340396523476</v>
       </c>
       <c r="G19" t="n">
         <v>105</v>
@@ -896,7 +896,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6390115320682526</v>
+        <v>0.9906089622527361</v>
       </c>
       <c r="G20" t="n">
         <v>199</v>
@@ -919,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>0.7952219992876053</v>
+        <v>0.9936257107183337</v>
       </c>
       <c r="G21" t="n">
         <v>139</v>
@@ -942,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>0.6987122297286987</v>
+        <v>0.9977231787052006</v>
       </c>
       <c r="G22" t="n">
         <v>98</v>
@@ -965,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>0.8306220471858978</v>
+        <v>0.9950504712760448</v>
       </c>
       <c r="G23" t="n">
         <v>147</v>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>0.7306775748729706</v>
+        <v>0.9988517602905631</v>
       </c>
       <c r="G24" t="n">
         <v>66</v>
@@ -1011,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>0.8210077285766602</v>
+        <v>0.9914289759472013</v>
       </c>
       <c r="G25" t="n">
         <v>97</v>
@@ -1034,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>0.8648902326822281</v>
+        <v>0.9459285624325275</v>
       </c>
       <c r="G26" t="n">
         <v>93</v>
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9764693789184093</v>
+        <v>0.9946284284815192</v>
       </c>
       <c r="G27" t="n">
         <v>15</v>
@@ -1080,7 +1080,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>0.8546960949897766</v>
+        <v>0.9773000385612249</v>
       </c>
       <c r="G28" t="n">
         <v>56</v>
@@ -1103,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>0.8198293447494507</v>
+        <v>0.9887322187423706</v>
       </c>
       <c r="G29" t="n">
         <v>4</v>
@@ -1126,7 +1126,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9307363033294678</v>
+        <v>0.9919607043266296</v>
       </c>
       <c r="G30" t="n">
         <v>4</v>
@@ -1149,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>0.9142290949821472</v>
+        <v>0.9917110204696655</v>
       </c>
       <c r="G31" t="n">
         <v>3</v>
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>0.8812274932861328</v>
+        <v>0.9973405003547668</v>
       </c>
       <c r="G32" t="n">
         <v>2</v>
@@ -1195,7 +1195,7 @@
         <v>1</v>
       </c>
       <c r="F33" t="n">
-        <v>0.954254150390625</v>
+        <v>0.9956170320510864</v>
       </c>
       <c r="G33" t="n">
         <v>4</v>
@@ -1218,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>0.8780286312103271</v>
+        <v>0.997776210308075</v>
       </c>
       <c r="G34" t="n">
         <v>3</v>
@@ -1241,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9682930111885071</v>
+        <v>0.9933363199234009</v>
       </c>
       <c r="G35" t="n">
         <v>2</v>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9885011911392212</v>
+        <v>0.9984061121940613</v>
       </c>
       <c r="G36" t="n">
         <v>4</v>
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>0.9496772289276123</v>
+        <v>0.9940755367279053</v>
       </c>
       <c r="G37" t="n">
         <v>3</v>
@@ -1310,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>0.9781948924064636</v>
+        <v>0.9967204928398132</v>
       </c>
       <c r="G38" t="n">
         <v>4</v>
@@ -1333,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>0.9740368723869324</v>
+        <v>0.9871864318847656</v>
       </c>
       <c r="G39" t="n">
         <v>4</v>
@@ -1356,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>0.8501008152961731</v>
+        <v>0.9973031282424927</v>
       </c>
       <c r="G40" t="n">
         <v>4</v>
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="F41" t="n">
-        <v>0.9538899064064026</v>
+        <v>0.9910684823989868</v>
       </c>
       <c r="G41" t="n">
         <v>3</v>
@@ -1402,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9162575602531433</v>
+        <v>0.9972319006919861</v>
       </c>
       <c r="G42" t="n">
         <v>4</v>
@@ -1425,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>0.9669449329376221</v>
+        <v>0.9948580265045166</v>
       </c>
       <c r="G43" t="n">
         <v>3</v>
@@ -1448,7 +1448,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="n">
-        <v>0.8394485712051392</v>
+        <v>0.996832549571991</v>
       </c>
       <c r="G44" t="n">
         <v>4</v>
@@ -1471,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="n">
-        <v>0.902647852897644</v>
+        <v>0.9881040453910828</v>
       </c>
       <c r="G45" t="n">
         <v>3</v>
@@ -1494,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>0.8512742519378662</v>
+        <v>0.9783088564872742</v>
       </c>
       <c r="G46" t="n">
         <v>3</v>
@@ -1517,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>0.6232940554618835</v>
+        <v>0.9940879344940186</v>
       </c>
       <c r="G47" t="n">
         <v>2</v>
@@ -1540,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="F48" t="n">
-        <v>0.9672390818595886</v>
+        <v>0.9962377548217773</v>
       </c>
       <c r="G48" t="n">
         <v>4</v>
@@ -1563,7 +1563,7 @@
         <v>1</v>
       </c>
       <c r="F49" t="n">
-        <v>0.751841127872467</v>
+        <v>0.9968886971473694</v>
       </c>
       <c r="G49" t="n">
         <v>3</v>
@@ -1586,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="F50" t="n">
-        <v>0.9387869834899902</v>
+        <v>0.9887853860855103</v>
       </c>
       <c r="G50" t="n">
         <v>2</v>
@@ -1609,7 +1609,7 @@
         <v>1</v>
       </c>
       <c r="F51" t="n">
-        <v>0.930402934551239</v>
+        <v>0.9668812155723572</v>
       </c>
       <c r="G51" t="n">
         <v>4</v>
@@ -1632,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="n">
-        <v>0.9053544402122498</v>
+        <v>0.984312891960144</v>
       </c>
       <c r="G52" t="n">
         <v>3</v>
@@ -1655,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>0.8165971636772156</v>
+        <v>0.9976372718811035</v>
       </c>
       <c r="G53" t="n">
         <v>4</v>
@@ -1678,7 +1678,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="n">
-        <v>0.8856334686279297</v>
+        <v>0.9993595480918884</v>
       </c>
       <c r="G54" t="n">
         <v>3</v>
@@ -1701,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="F55" t="n">
-        <v>0.7622784376144409</v>
+        <v>0.9958695769309998</v>
       </c>
       <c r="G55" t="n">
         <v>4</v>
@@ -1724,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="F56" t="n">
-        <v>0.9138050675392151</v>
+        <v>0.9898996949195862</v>
       </c>
       <c r="G56" t="n">
         <v>3</v>
@@ -1747,7 +1747,7 @@
         <v>1</v>
       </c>
       <c r="F57" t="n">
-        <v>0.9069384932518005</v>
+        <v>0.9982284903526306</v>
       </c>
       <c r="G57" t="n">
         <v>4</v>
@@ -1770,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="F58" t="n">
-        <v>0.9721471071243286</v>
+        <v>0.996516227722168</v>
       </c>
       <c r="G58" t="n">
         <v>3</v>
@@ -1793,7 +1793,7 @@
         <v>1</v>
       </c>
       <c r="F59" t="n">
-        <v>0.6264758706092834</v>
+        <v>0.9474180340766907</v>
       </c>
       <c r="G59" t="n">
         <v>4</v>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
       <c r="F60" t="n">
-        <v>0.9413217902183533</v>
+        <v>0.9950710535049438</v>
       </c>
       <c r="G60" t="n">
         <v>3</v>
@@ -1839,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="n">
-        <v>0.6988458037376404</v>
+        <v>0.978162944316864</v>
       </c>
       <c r="G61" t="n">
         <v>2</v>
@@ -1862,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="F62" t="n">
-        <v>0.8964338898658752</v>
+        <v>0.9992918968200684</v>
       </c>
       <c r="G62" t="n">
         <v>4</v>
@@ -1885,7 +1885,7 @@
         <v>1</v>
       </c>
       <c r="F63" t="n">
-        <v>0.8250556588172913</v>
+        <v>0.9973828196525574</v>
       </c>
       <c r="G63" t="n">
         <v>4</v>
@@ -1908,7 +1908,7 @@
         <v>1</v>
       </c>
       <c r="F64" t="n">
-        <v>0.6630588173866272</v>
+        <v>0.9925822019577026</v>
       </c>
       <c r="G64" t="n">
         <v>3</v>
@@ -1931,7 +1931,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="n">
-        <v>0.9651884436607361</v>
+        <v>0.9919629096984863</v>
       </c>
       <c r="G65" t="n">
         <v>4</v>
@@ -1954,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="F66" t="n">
-        <v>0.74409019947052</v>
+        <v>0.9925715327262878</v>
       </c>
       <c r="G66" t="n">
         <v>3</v>
@@ -1977,7 +1977,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="n">
-        <v>0.8486421704292297</v>
+        <v>0.9977922439575195</v>
       </c>
       <c r="G67" t="n">
         <v>2</v>
@@ -2000,7 +2000,7 @@
         <v>1</v>
       </c>
       <c r="F68" t="n">
-        <v>0.7397407293319702</v>
+        <v>0.9661133885383606</v>
       </c>
       <c r="G68" t="n">
         <v>4</v>
@@ -2023,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="F69" t="n">
-        <v>0.9573210477828979</v>
+        <v>0.9857527613639832</v>
       </c>
       <c r="G69" t="n">
         <v>3</v>
@@ -2046,7 +2046,7 @@
         <v>1</v>
       </c>
       <c r="F70" t="n">
-        <v>0.9564624428749084</v>
+        <v>0.9939227700233459</v>
       </c>
       <c r="G70" t="n">
         <v>4</v>
@@ -2069,7 +2069,7 @@
         <v>1</v>
       </c>
       <c r="F71" t="n">
-        <v>0.9109674096107483</v>
+        <v>0.9989321827888489</v>
       </c>
       <c r="G71" t="n">
         <v>3</v>
@@ -2092,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="n">
-        <v>0.767642617225647</v>
+        <v>0.9598271250724792</v>
       </c>
       <c r="G72" t="n">
         <v>4</v>
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="F73" t="n">
-        <v>0.8574867844581604</v>
+        <v>0.9753674864768982</v>
       </c>
       <c r="G73" t="n">
         <v>4</v>
@@ -2138,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="F74" t="n">
-        <v>0.9239479899406433</v>
+        <v>0.9857174158096313</v>
       </c>
       <c r="G74" t="n">
         <v>3</v>
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="F75" t="n">
-        <v>0.8656856417655945</v>
+        <v>0.9984306693077087</v>
       </c>
       <c r="G75" t="n">
         <v>3</v>
@@ -2184,7 +2184,7 @@
         <v>1</v>
       </c>
       <c r="F76" t="n">
-        <v>0.9259476661682129</v>
+        <v>0.9947405457496643</v>
       </c>
       <c r="G76" t="n">
         <v>4</v>
@@ -2207,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="F77" t="n">
-        <v>0.9150565266609192</v>
+        <v>0.993002712726593</v>
       </c>
       <c r="G77" t="n">
         <v>4</v>
@@ -2230,7 +2230,7 @@
         <v>1</v>
       </c>
       <c r="F78" t="n">
-        <v>0.9774895310401917</v>
+        <v>0.9848284125328064</v>
       </c>
       <c r="G78" t="n">
         <v>3</v>
@@ -2253,7 +2253,7 @@
         <v>1</v>
       </c>
       <c r="F79" t="n">
-        <v>0.9847817420959473</v>
+        <v>0.9989218711853027</v>
       </c>
       <c r="G79" t="n">
         <v>2</v>
@@ -2276,7 +2276,7 @@
         <v>1</v>
       </c>
       <c r="F80" t="n">
-        <v>0.7749574184417725</v>
+        <v>0.9986732006072998</v>
       </c>
       <c r="G80" t="n">
         <v>4</v>
@@ -2299,7 +2299,7 @@
         <v>1</v>
       </c>
       <c r="F81" t="n">
-        <v>0.7927783131599426</v>
+        <v>0.9975624084472656</v>
       </c>
       <c r="G81" t="n">
         <v>3</v>
@@ -2322,7 +2322,7 @@
         <v>1</v>
       </c>
       <c r="F82" t="n">
-        <v>0.9366551041603088</v>
+        <v>0.9972395896911621</v>
       </c>
       <c r="G82" t="n">
         <v>4</v>
@@ -2345,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="F83" t="n">
-        <v>0.9410690069198608</v>
+        <v>0.9973642230033875</v>
       </c>
       <c r="G83" t="n">
         <v>4</v>
@@ -2368,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="F84" t="n">
-        <v>0.930187463760376</v>
+        <v>0.9867449402809143</v>
       </c>
       <c r="G84" t="n">
         <v>3</v>
@@ -2391,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="F85" t="n">
-        <v>0.9564469456672668</v>
+        <v>0.9921119213104248</v>
       </c>
       <c r="G85" t="n">
         <v>4</v>
@@ -2414,7 +2414,7 @@
         <v>1</v>
       </c>
       <c r="F86" t="n">
-        <v>0.9367327094078064</v>
+        <v>0.9978207349777222</v>
       </c>
       <c r="G86" t="n">
         <v>3</v>
@@ -2431,13 +2431,13 @@
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
-        <v>0.5267112255096436</v>
+        <v>0.8810082376003265</v>
       </c>
       <c r="G87" t="n">
         <v>137</v>
@@ -2460,7 +2460,7 @@
         <v>1</v>
       </c>
       <c r="F88" t="n">
-        <v>0.6881051361560822</v>
+        <v>0.9901557229459286</v>
       </c>
       <c r="G88" t="n">
         <v>125</v>
@@ -2483,7 +2483,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="n">
-        <v>0.7993205189704895</v>
+        <v>0.9989523759577423</v>
       </c>
       <c r="G89" t="n">
         <v>48</v>
@@ -2500,13 +2500,13 @@
         <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>0.6696648299694061</v>
+        <v>0.9738199710845947</v>
       </c>
       <c r="G90" t="n">
         <v>46</v>
@@ -2529,7 +2529,7 @@
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>0.67120760679245</v>
+        <v>0.9438732266426086</v>
       </c>
       <c r="G91" t="n">
         <v>138</v>
@@ -2546,13 +2546,13 @@
         <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
-        <v>0.9344892501831055</v>
+        <v>0.6744269132614136</v>
       </c>
       <c r="G92" t="n">
         <v>146</v>
@@ -2569,13 +2569,13 @@
         <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>0.8812622651457787</v>
+        <v>0.8503650426864624</v>
       </c>
       <c r="G93" t="n">
         <v>60</v>
@@ -2598,7 +2598,7 @@
         <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>0.9696806073188782</v>
+        <v>0.9237037301063538</v>
       </c>
       <c r="G94" t="n">
         <v>101</v>
@@ -2615,13 +2615,13 @@
         <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95" t="n">
-        <v>0.6207723319530487</v>
+        <v>0.9886132478713989</v>
       </c>
       <c r="G95" t="n">
         <v>148</v>
@@ -2638,13 +2638,13 @@
         <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
-        <v>0.9384464025497437</v>
+        <v>0.5722082853317261</v>
       </c>
       <c r="G96" t="n">
         <v>140</v>
@@ -2667,7 +2667,7 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>0.8498570322990417</v>
+        <v>0.8486617207527161</v>
       </c>
       <c r="G97" t="n">
         <v>114</v>
@@ -2684,13 +2684,13 @@
         <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>0.7683752775192261</v>
+        <v>0.6089860200881958</v>
       </c>
       <c r="G98" t="n">
         <v>29</v>
@@ -2713,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>0.9315692782402039</v>
+        <v>0.67630934715271</v>
       </c>
       <c r="G99" t="n">
         <v>40</v>
@@ -2736,7 +2736,7 @@
         <v>1</v>
       </c>
       <c r="F100" t="n">
-        <v>0.8109794557094574</v>
+        <v>0.9806087203323841</v>
       </c>
       <c r="G100" t="n">
         <v>127</v>
@@ -2753,13 +2753,13 @@
         <v>0</v>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" t="n">
-        <v>0.9761126637458801</v>
+        <v>0.8542082756757736</v>
       </c>
       <c r="G101" t="n">
         <v>114</v>
@@ -2776,13 +2776,13 @@
         <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E102" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>0.7256071269512177</v>
+        <v>0.9458279013633728</v>
       </c>
       <c r="G102" t="n">
         <v>130</v>
@@ -2805,7 +2805,7 @@
         <v>1</v>
       </c>
       <c r="F103" t="n">
-        <v>0.5622592568397522</v>
+        <v>0.8669256567955017</v>
       </c>
       <c r="G103" t="n">
         <v>94</v>
@@ -2822,13 +2822,13 @@
         <v>0</v>
       </c>
       <c r="D104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104" t="n">
-        <v>0.8707664608955383</v>
+        <v>0.9819917995482683</v>
       </c>
       <c r="G104" t="n">
         <v>65</v>
@@ -2851,7 +2851,7 @@
         <v>1</v>
       </c>
       <c r="F105" t="n">
-        <v>0.8349959552288055</v>
+        <v>0.9098582714796066</v>
       </c>
       <c r="G105" t="n">
         <v>54</v>
@@ -2868,13 +2868,13 @@
         <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F106" t="n">
-        <v>0.618441641330719</v>
+        <v>0.5959334671497345</v>
       </c>
       <c r="G106" t="n">
         <v>111</v>
@@ -2891,13 +2891,13 @@
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F107" t="n">
-        <v>0.8470392674207687</v>
+        <v>0.9210028052330017</v>
       </c>
       <c r="G107" t="n">
         <v>49</v>
@@ -2920,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="F108" t="n">
-        <v>0.6346876323223114</v>
+        <v>0.9449789710342884</v>
       </c>
       <c r="G108" t="n">
         <v>47</v>
@@ -2943,7 +2943,7 @@
         <v>1</v>
       </c>
       <c r="F109" t="n">
-        <v>0.8714707940816879</v>
+        <v>0.8336544632911682</v>
       </c>
       <c r="G109" t="n">
         <v>96</v>
@@ -2960,13 +2960,13 @@
         <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110" t="n">
-        <v>0.8009137511253357</v>
+        <v>0.9248353466391563</v>
       </c>
       <c r="G110" t="n">
         <v>37</v>
@@ -2989,7 +2989,7 @@
         <v>1</v>
       </c>
       <c r="F111" t="n">
-        <v>0.6181081831455231</v>
+        <v>0.6510941982269287</v>
       </c>
       <c r="G111" t="n">
         <v>119</v>
@@ -3012,7 +3012,7 @@
         <v>1</v>
       </c>
       <c r="F112" t="n">
-        <v>0.6917822957038879</v>
+        <v>0.7108362913131714</v>
       </c>
       <c r="G112" t="n">
         <v>102</v>

</xml_diff>